<commit_message>
Small changes to model
</commit_message>
<xml_diff>
--- a/given_data/demanddata.xlsx
+++ b/given_data/demanddata.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/l_martin_tue_nl/Documents/Transportation Teaching/1CM110/2022/Block 2/Assignment/Shared Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c0012dffc44a574/Documents/Masters/TUe/Q2/Descion Making/Assignment/Assignment 2/DecisionMaking_Assignment_3/given_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{142E956A-9A19-4498-8FF1-5468F5D5E3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F5CD016-BA68-44C9-B077-A3A7B21FAEF0}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{142E956A-9A19-4498-8FF1-5468F5D5E3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D4A954A-BB1A-4B81-89C5-1102D47DFD04}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-1965" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -160,7 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -441,12 +452,17 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +509,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -507,7 +523,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -524,7 +540,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -535,7 +551,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -546,7 +562,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -557,7 +573,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -568,7 +584,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -579,7 +595,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -590,7 +606,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -616,7 +632,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -642,7 +658,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -668,7 +684,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -694,7 +710,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>

</xml_diff>